<commit_message>
Added "Ser/Bld" to the "Intravascular- Any" grouper
</commit_message>
<xml_diff>
--- a/class_CHEM/lists.xlsx
+++ b/class_CHEM/lists.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\Windows_plynch\Documents\NLM\Projects\LOINC equivalence classes\Chemistry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\project\LOINC-equivalence-classes\class_CHEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="56">
   <si>
     <t>LIST_NAME</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>Bld O2 Peak</t>
+  </si>
+  <si>
+    <t>Ser/Bld</t>
   </si>
 </sst>
 </file>
@@ -518,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1077,7 @@
         <v>53</v>
       </c>
       <c r="D39" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1088,7 +1091,7 @@
         <v>53</v>
       </c>
       <c r="D40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1102,7 +1105,7 @@
         <v>53</v>
       </c>
       <c r="D41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1116,7 +1119,7 @@
         <v>53</v>
       </c>
       <c r="D42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1126,11 +1129,11 @@
       <c r="B43" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>54</v>
+      <c r="C43" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1144,6 +1147,20 @@
         <v>54</v>
       </c>
       <c r="D44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>